<commit_message>
Adiciona lancamento futuro e funcao DiasParaLancamento
</commit_message>
<xml_diff>
--- a/M_DiagramaFisico.xlsx
+++ b/M_DiagramaFisico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34132336883\Desktop\SENAI\GitHub\2s2019-sprint-1-bd-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFAA9B3-6B4D-4881-9A84-A7EAB144B305}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD108F1A-7464-4EA9-8DB0-7CFC61443E2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="5955" xr2:uid="{F8CC6F07-69E4-4704-AA72-9860FF096584}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
   <si>
     <t>OpFlix</t>
   </si>
@@ -232,13 +232,19 @@
   </si>
   <si>
     <t>Veiculos</t>
+  </si>
+  <si>
+    <t>Alladin</t>
+  </si>
+  <si>
+    <t>Um jovem árabe que se apaixona por uma princesa e para conquistá-la conta com a ajuda de um gênio da lâmpada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,6 +271,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -404,7 +418,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -448,6 +462,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -765,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6CC6CAA-40F2-42FF-AA21-32FDB28ABAF1}">
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="D14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,7 +1292,7 @@
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>37</v>
       </c>
@@ -1290,7 +1305,7 @@
       <c r="H34" s="18"/>
       <c r="I34" s="18"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>38</v>
       </c>
@@ -1319,7 +1334,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>1</v>
       </c>
@@ -1348,7 +1363,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>2</v>
       </c>
@@ -1377,7 +1392,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>3</v>
       </c>
@@ -1406,7 +1421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>4</v>
       </c>
@@ -1435,24 +1450,40 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>5</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" s="8">
+        <v>102</v>
+      </c>
+      <c r="E40" s="9">
+        <v>43711</v>
+      </c>
+      <c r="F40" s="8">
+        <v>5</v>
+      </c>
+      <c r="G40" s="8">
+        <v>2</v>
+      </c>
+      <c r="H40" s="8">
+        <v>1</v>
+      </c>
+      <c r="I40" s="8">
+        <v>3</v>
+      </c>
+      <c r="J40" s="23"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>6</v>
       </c>
-      <c r="B41" s="5"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
@@ -1461,7 +1492,7 @@
       <c r="H41" s="8"/>
       <c r="I41" s="8"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>7</v>
       </c>

</xml_diff>